<commit_message>
Fixed data entry errors; denominator changes between studies
</commit_message>
<xml_diff>
--- a/OR_compendium.xlsx
+++ b/OR_compendium.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="21060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overall.OR" sheetId="1" r:id="rId1"/>
@@ -1268,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1309,7 +1309,7 @@
         <v>26</v>
       </c>
       <c r="C2">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>331</v>
@@ -1472,13 +1472,13 @@
         <v>16</v>
       </c>
       <c r="D10">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
       <c r="F10">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1532,13 +1532,13 @@
         <v>64</v>
       </c>
       <c r="D13">
-        <v>1313</v>
+        <v>1317</v>
       </c>
       <c r="E13">
         <v>23</v>
       </c>
       <c r="F13">
-        <v>677</v>
+        <v>686</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1552,7 +1552,7 @@
         <v>4</v>
       </c>
       <c r="D14">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -1578,7 +1578,7 @@
         <v>7</v>
       </c>
       <c r="F15">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1612,7 +1612,7 @@
         <v>39</v>
       </c>
       <c r="D17">
-        <v>1313</v>
+        <v>1307</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -2112,10 +2112,10 @@
         <v>17</v>
       </c>
       <c r="D42">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>161</v>
       </c>
       <c r="F42">
         <v>165</v>
@@ -2132,13 +2132,13 @@
         <v>3</v>
       </c>
       <c r="D43">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="E43">
         <v>2</v>
       </c>
       <c r="F43">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2152,13 +2152,13 @@
         <v>3</v>
       </c>
       <c r="D44">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2172,13 +2172,13 @@
         <v>40</v>
       </c>
       <c r="D45">
-        <v>1313</v>
+        <v>1315</v>
       </c>
       <c r="E45">
         <v>19</v>
       </c>
       <c r="F45">
-        <v>677</v>
+        <v>682</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2192,13 +2192,13 @@
         <v>2</v>
       </c>
       <c r="D46">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2212,13 +2212,13 @@
         <v>2</v>
       </c>
       <c r="D47">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2232,13 +2232,13 @@
         <v>0</v>
       </c>
       <c r="D48">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2252,13 +2252,13 @@
         <v>12</v>
       </c>
       <c r="D49">
-        <v>1313</v>
+        <v>1315</v>
       </c>
       <c r="E49">
         <v>8</v>
       </c>
       <c r="F49">
-        <v>677</v>
+        <v>682</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2272,7 +2272,7 @@
         <v>3</v>
       </c>
       <c r="D50">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2298,7 +2298,7 @@
         <v>2</v>
       </c>
       <c r="F51">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2332,7 +2332,7 @@
         <v>50</v>
       </c>
       <c r="D53">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="E53">
         <v>18</v>
@@ -2592,13 +2592,13 @@
         <v>3</v>
       </c>
       <c r="D66">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2618,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2632,7 +2632,7 @@
         <v>4</v>
       </c>
       <c r="D68">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E68">
         <v>2</v>
@@ -2652,13 +2652,13 @@
         <v>20</v>
       </c>
       <c r="D69">
-        <v>1313</v>
+        <v>1301</v>
       </c>
       <c r="E69">
         <v>5</v>
       </c>
       <c r="F69">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2669,16 +2669,16 @@
         <v>26</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D70">
-        <v>331</v>
+        <v>239</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2698,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2712,7 +2712,7 @@
         <v>4</v>
       </c>
       <c r="D72">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2732,13 +2732,13 @@
         <v>18</v>
       </c>
       <c r="D73">
-        <v>1313</v>
+        <v>1301</v>
       </c>
       <c r="E73">
         <v>5</v>
       </c>
       <c r="F73">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2752,13 +2752,13 @@
         <v>1</v>
       </c>
       <c r="D74">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2778,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2792,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -2812,13 +2812,13 @@
         <v>2</v>
       </c>
       <c r="D77">
-        <v>1313</v>
+        <v>1301</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2832,13 +2832,13 @@
         <v>2</v>
       </c>
       <c r="D78">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="F78">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2858,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="F79">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2892,13 +2892,13 @@
         <v>14</v>
       </c>
       <c r="D81">
-        <v>1313</v>
+        <v>1315</v>
       </c>
       <c r="E81">
         <v>5</v>
       </c>
       <c r="F81">
-        <v>677</v>
+        <v>686</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2912,13 +2912,13 @@
         <v>1</v>
       </c>
       <c r="D82">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="F82">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2938,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2952,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="D84">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -2972,13 +2972,13 @@
         <v>6</v>
       </c>
       <c r="D85">
-        <v>1313</v>
+        <v>1299</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>